<commit_message>
Update 2. Conditional Formatting - Exercise.xlsx
</commit_message>
<xml_diff>
--- a/2. Conditional Formatting - Exercise.xlsx
+++ b/2. Conditional Formatting - Exercise.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27031"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27108"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alphad.sharepoint.com/sites/Clients/Shared Documents/HSBC/2023/12199 - HSBC EMEA - Excel Training Sheffield Grads 2023/Materials/Session 3- Enhancing Your Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GeorgeMount\Documents\GitHub\hsbc-enhancing-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{6A816880-AD52-463D-AACD-2E1A27B7CD8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{228506DF-C2A9-45D1-ADFA-DCCFAE760FB4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA9891A-CEED-46A0-A33E-475515933AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="18915" windowHeight="12676" xr2:uid="{5CAEE100-183E-4775-BB86-11B5C6F85569}"/>
+    <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="16395" xr2:uid="{5CAEE100-183E-4775-BB86-11B5C6F85569}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
   <si>
     <t>When you are ready, unhide the ANSWERS worksheet for answers and examples.</t>
   </si>
@@ -122,48 +122,13 @@
     <t>1. Add a heatmap to the table below. Be careful in your choice of color palette.</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Up/Down arrows can be found in </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Icon Sets &gt; Directional</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. Select a row: Excel assumes a continuous series running left to right.</t>
-    </r>
-  </si>
-  <si>
-    <t>|</t>
-  </si>
-  <si>
-    <t xml:space="preserve">| Your manager has defined the breakeven point for working with a client as 100 per </t>
-  </si>
-  <si>
-    <t>| month. Here the rule flags numbers less than that figure.</t>
-  </si>
-  <si>
-    <t>2. Make a copy of the table. This time, add other enhamcments you feel will add more impact to the data, such as sparklines.</t>
-  </si>
-  <si>
     <t>Sparkline</t>
   </si>
   <si>
     <t>(see below for more)</t>
+  </si>
+  <si>
+    <t>2. Add other enhancements you feel will add more impact to the data, such as sparklines.</t>
   </si>
 </sst>
 </file>
@@ -292,18 +257,7 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{38D2D0BF-3F13-4DF9-A9F6-12FB93C3C862}"/>
   </tableStyles>
@@ -676,9 +630,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="C2:P29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -694,7 +646,7 @@
     </row>
     <row r="3" spans="3:16" x14ac:dyDescent="0.45">
       <c r="C3" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="3:16" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
@@ -720,51 +672,51 @@
       </c>
       <c r="D8" s="6">
         <f t="shared" ref="D8:M8" ca="1" si="0">EDATE(E8,-1)</f>
-        <v>44908</v>
+        <v>44910</v>
       </c>
       <c r="E8" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>44939</v>
+        <v>44941</v>
       </c>
       <c r="F8" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>44970</v>
+        <v>44972</v>
       </c>
       <c r="G8" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>44998</v>
+        <v>45000</v>
       </c>
       <c r="H8" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45029</v>
+        <v>45031</v>
       </c>
       <c r="I8" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45059</v>
+        <v>45061</v>
       </c>
       <c r="J8" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45090</v>
+        <v>45092</v>
       </c>
       <c r="K8" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45120</v>
+        <v>45122</v>
       </c>
       <c r="L8" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45151</v>
+        <v>45153</v>
       </c>
       <c r="M8" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45182</v>
+        <v>45184</v>
       </c>
       <c r="N8" s="6">
         <f ca="1">EDATE(O8,-1)</f>
-        <v>45212</v>
+        <v>45214</v>
       </c>
       <c r="O8" s="6">
         <f ca="1">TODAY()</f>
-        <v>45243</v>
+        <v>45245</v>
       </c>
       <c r="P8" s="5" t="s">
         <v>2</v>
@@ -1702,10 +1654,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63ADEA5F-0768-4346-BD35-389C897097A2}">
-  <dimension ref="C2:S56"/>
+  <dimension ref="C2:S29"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B4" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="R40" sqref="R40"/>
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1722,14 +1674,17 @@
     </row>
     <row r="3" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C3" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="3:17" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C4" s="2"/>
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="3:17" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="3:17" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C6" s="2"/>
@@ -1745,57 +1700,57 @@
       </c>
       <c r="D8" s="6">
         <f t="shared" ref="D8:M8" ca="1" si="0">EDATE(E8,-1)</f>
-        <v>44908</v>
+        <v>44910</v>
       </c>
       <c r="E8" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>44939</v>
+        <v>44941</v>
       </c>
       <c r="F8" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>44970</v>
+        <v>44972</v>
       </c>
       <c r="G8" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>44998</v>
+        <v>45000</v>
       </c>
       <c r="H8" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45029</v>
+        <v>45031</v>
       </c>
       <c r="I8" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45059</v>
+        <v>45061</v>
       </c>
       <c r="J8" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45090</v>
+        <v>45092</v>
       </c>
       <c r="K8" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45120</v>
+        <v>45122</v>
       </c>
       <c r="L8" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45151</v>
+        <v>45153</v>
       </c>
       <c r="M8" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45182</v>
+        <v>45184</v>
       </c>
       <c r="N8" s="6">
         <f ca="1">EDATE(O8,-1)</f>
-        <v>45212</v>
+        <v>45214</v>
       </c>
       <c r="O8" s="6">
         <f ca="1">TODAY()</f>
-        <v>45243</v>
+        <v>45245</v>
       </c>
       <c r="P8" s="5" t="s">
         <v>2</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="3:17" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
@@ -2742,1018 +2697,10 @@
         <v>49580.453040608554</v>
       </c>
       <c r="S29" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="3:18" x14ac:dyDescent="0.45">
-      <c r="C34" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="35" spans="3:18" x14ac:dyDescent="0.45">
-      <c r="C35" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D35" s="6">
-        <f t="shared" ref="D35:M35" ca="1" si="1">EDATE(E35,-1)</f>
-        <v>44908</v>
-      </c>
-      <c r="E35" s="6">
-        <f t="shared" ca="1" si="1"/>
-        <v>44939</v>
-      </c>
-      <c r="F35" s="6">
-        <f t="shared" ca="1" si="1"/>
-        <v>44970</v>
-      </c>
-      <c r="G35" s="6">
-        <f t="shared" ca="1" si="1"/>
-        <v>44998</v>
-      </c>
-      <c r="H35" s="6">
-        <f t="shared" ca="1" si="1"/>
-        <v>45029</v>
-      </c>
-      <c r="I35" s="6">
-        <f t="shared" ca="1" si="1"/>
-        <v>45059</v>
-      </c>
-      <c r="J35" s="6">
-        <f t="shared" ca="1" si="1"/>
-        <v>45090</v>
-      </c>
-      <c r="K35" s="6">
-        <f t="shared" ca="1" si="1"/>
-        <v>45120</v>
-      </c>
-      <c r="L35" s="6">
-        <f t="shared" ca="1" si="1"/>
-        <v>45151</v>
-      </c>
-      <c r="M35" s="6">
-        <f t="shared" ca="1" si="1"/>
-        <v>45182</v>
-      </c>
-      <c r="N35" s="6">
-        <f ca="1">EDATE(O35,-1)</f>
-        <v>45212</v>
-      </c>
-      <c r="O35" s="6">
-        <f ca="1">TODAY()</f>
-        <v>45243</v>
-      </c>
-      <c r="P35" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="3:18" x14ac:dyDescent="0.45">
-      <c r="C36" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D36" s="7">
-        <v>339.64013294442009</v>
-      </c>
-      <c r="E36" s="7">
-        <v>300.88496388694006</v>
-      </c>
-      <c r="F36" s="7">
-        <v>326.36525067603009</v>
-      </c>
-      <c r="G36" s="7">
-        <v>282.96022426032999</v>
-      </c>
-      <c r="H36" s="7">
-        <v>331.67979573758998</v>
-      </c>
-      <c r="I36" s="7">
-        <v>305.72480309181003</v>
-      </c>
-      <c r="J36" s="7">
-        <v>350.11762245759019</v>
-      </c>
-      <c r="K36" s="7">
-        <v>236.50374681387004</v>
-      </c>
-      <c r="L36" s="7">
-        <v>271.22782381146004</v>
-      </c>
-      <c r="M36" s="7">
-        <v>279.02641284801996</v>
-      </c>
-      <c r="N36" s="7">
-        <v>283.52997054252</v>
-      </c>
-      <c r="O36" s="7">
-        <v>196.29269970978999</v>
-      </c>
-      <c r="P36" s="4">
-        <v>3503.9534467803696</v>
-      </c>
-      <c r="R36" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="37" spans="3:18" x14ac:dyDescent="0.45">
-      <c r="C37" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D37" s="7">
-        <v>75.562346552219992</v>
-      </c>
-      <c r="E37" s="7">
-        <v>99.059965851030015</v>
-      </c>
-      <c r="F37" s="7">
-        <v>90.210039447400007</v>
-      </c>
-      <c r="G37" s="7">
-        <v>59.820002317790014</v>
-      </c>
-      <c r="H37" s="7">
-        <v>73.777264619020031</v>
-      </c>
-      <c r="I37" s="7">
-        <v>84.269969667930013</v>
-      </c>
-      <c r="J37" s="7">
-        <v>69.502152479700001</v>
-      </c>
-      <c r="K37" s="7">
-        <v>58.159989839059996</v>
-      </c>
-      <c r="L37" s="7">
-        <v>0</v>
-      </c>
-      <c r="M37" s="7">
-        <v>0</v>
-      </c>
-      <c r="N37" s="7">
-        <v>0</v>
-      </c>
-      <c r="O37" s="7">
-        <v>0</v>
-      </c>
-      <c r="P37" s="4">
-        <v>610.36173077415015</v>
-      </c>
-      <c r="R37" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="38" spans="3:18" x14ac:dyDescent="0.45">
-      <c r="C38" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" s="7">
-        <v>244.35955477390007</v>
-      </c>
-      <c r="E38" s="7">
-        <v>248.85494464704996</v>
-      </c>
-      <c r="F38" s="7">
-        <v>333.77020934791994</v>
-      </c>
-      <c r="G38" s="7">
-        <v>203.06350740612001</v>
-      </c>
-      <c r="H38" s="7">
-        <v>280.11987819129996</v>
-      </c>
-      <c r="I38" s="7">
-        <v>249.7398402524</v>
-      </c>
-      <c r="J38" s="7">
-        <v>197.24003280466005</v>
-      </c>
-      <c r="K38" s="7">
-        <v>218.97209873605996</v>
-      </c>
-      <c r="L38" s="7">
-        <v>222.11494389598997</v>
-      </c>
-      <c r="M38" s="7">
-        <v>223.66278002903005</v>
-      </c>
-      <c r="N38" s="7">
-        <v>159.93679681861005</v>
-      </c>
-      <c r="O38" s="7">
-        <v>87.390140945539983</v>
-      </c>
-      <c r="P38" s="4">
-        <v>2669.2247278485802</v>
-      </c>
-      <c r="R38" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="39" spans="3:18" x14ac:dyDescent="0.45">
-      <c r="C39" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="7">
-        <v>380.81058340590005</v>
-      </c>
-      <c r="E39" s="7">
-        <v>266.31841377334007</v>
-      </c>
-      <c r="F39" s="7">
-        <v>273.67000531047</v>
-      </c>
-      <c r="G39" s="7">
-        <v>285.99003943495006</v>
-      </c>
-      <c r="H39" s="7">
-        <v>241.95644885448002</v>
-      </c>
-      <c r="I39" s="7">
-        <v>312.29153780289994</v>
-      </c>
-      <c r="J39" s="7">
-        <v>250.11992075153003</v>
-      </c>
-      <c r="K39" s="7">
-        <v>197.80996998170005</v>
-      </c>
-      <c r="L39" s="7">
-        <v>321.18013074097979</v>
-      </c>
-      <c r="M39" s="7">
-        <v>324.21006872122013</v>
-      </c>
-      <c r="N39" s="7">
-        <v>207.30992673636001</v>
-      </c>
-      <c r="O39" s="7">
-        <v>97.550165645879986</v>
-      </c>
-      <c r="P39" s="4">
-        <v>3159.2172111597097</v>
-      </c>
-      <c r="R39" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="3:18" x14ac:dyDescent="0.45">
-      <c r="C40" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D40" s="7">
-        <v>318.40188134657006</v>
-      </c>
-      <c r="E40" s="7">
-        <v>287.96014083093985</v>
-      </c>
-      <c r="F40" s="7">
-        <v>200.16370743473996</v>
-      </c>
-      <c r="G40" s="7">
-        <v>185.18746408931995</v>
-      </c>
-      <c r="H40" s="7">
-        <v>219.76678738728003</v>
-      </c>
-      <c r="I40" s="7">
-        <v>215.38658507259998</v>
-      </c>
-      <c r="J40" s="7">
-        <v>205.14998719644998</v>
-      </c>
-      <c r="K40" s="7">
-        <v>241.85257364500001</v>
-      </c>
-      <c r="L40" s="7">
-        <v>185.30003810463</v>
-      </c>
-      <c r="M40" s="7">
-        <v>212.18005681704997</v>
-      </c>
-      <c r="N40" s="7">
-        <v>108.65995893461003</v>
-      </c>
-      <c r="O40" s="7">
-        <v>91.139965817490008</v>
-      </c>
-      <c r="P40" s="4">
-        <v>2471.1491466766802</v>
-      </c>
-      <c r="R40" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="41" spans="3:18" x14ac:dyDescent="0.45">
-      <c r="C41" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D41" s="7">
-        <v>102.53732557791001</v>
-      </c>
-      <c r="E41" s="7">
-        <v>86.040009205019999</v>
-      </c>
-      <c r="F41" s="7">
-        <v>86.335651843650055</v>
-      </c>
-      <c r="G41" s="7">
-        <v>111.57620066277002</v>
-      </c>
-      <c r="H41" s="7">
-        <v>111.95996147124002</v>
-      </c>
-      <c r="I41" s="7">
-        <v>92.25502262399003</v>
-      </c>
-      <c r="J41" s="7">
-        <v>92.881962231690011</v>
-      </c>
-      <c r="K41" s="7">
-        <v>103.87549293972005</v>
-      </c>
-      <c r="L41" s="7">
-        <v>98.250029070060023</v>
-      </c>
-      <c r="M41" s="7">
-        <v>82.710007854599993</v>
-      </c>
-      <c r="N41" s="7">
-        <v>58.60494981003</v>
-      </c>
-      <c r="O41" s="7">
-        <v>54.514946188970008</v>
-      </c>
-      <c r="P41" s="4">
-        <v>1081.5415594796502</v>
-      </c>
-      <c r="R41" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="42" spans="3:18" x14ac:dyDescent="0.45">
-      <c r="C42" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D42" s="7">
-        <v>216.62012222420995</v>
-      </c>
-      <c r="E42" s="7">
-        <v>248.76926332866995</v>
-      </c>
-      <c r="F42" s="7">
-        <v>257.74006465390994</v>
-      </c>
-      <c r="G42" s="7">
-        <v>259.16484746600003</v>
-      </c>
-      <c r="H42" s="7">
-        <v>201.48469244737004</v>
-      </c>
-      <c r="I42" s="7">
-        <v>191.68986469302999</v>
-      </c>
-      <c r="J42" s="7">
-        <v>220.11859038534001</v>
-      </c>
-      <c r="K42" s="7">
-        <v>237.66389058196995</v>
-      </c>
-      <c r="L42" s="7">
-        <v>236.70992767883996</v>
-      </c>
-      <c r="M42" s="7">
-        <v>251.55813641179995</v>
-      </c>
-      <c r="N42" s="7">
-        <v>171.10996786490998</v>
-      </c>
-      <c r="O42" s="7">
-        <v>100.97332697638001</v>
-      </c>
-      <c r="P42" s="4">
-        <v>2593.6026947124296</v>
-      </c>
-    </row>
-    <row r="43" spans="3:18" x14ac:dyDescent="0.45">
-      <c r="C43" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D43" s="7">
-        <v>220.18011256107999</v>
-      </c>
-      <c r="E43" s="7">
-        <v>244.69008341639</v>
-      </c>
-      <c r="F43" s="7">
-        <v>182.92339977700004</v>
-      </c>
-      <c r="G43" s="7">
-        <v>215.08245761222997</v>
-      </c>
-      <c r="H43" s="7">
-        <v>181.54711646671998</v>
-      </c>
-      <c r="I43" s="7">
-        <v>190.62528558066995</v>
-      </c>
-      <c r="J43" s="7">
-        <v>216.39692353094992</v>
-      </c>
-      <c r="K43" s="7">
-        <v>224.91014425276001</v>
-      </c>
-      <c r="L43" s="7">
-        <v>219.25010407256997</v>
-      </c>
-      <c r="M43" s="7">
-        <v>208.85442353912001</v>
-      </c>
-      <c r="N43" s="7">
-        <v>210.52998446325998</v>
-      </c>
-      <c r="O43" s="7">
-        <v>69.449976712959995</v>
-      </c>
-      <c r="P43" s="4">
-        <v>2384.4400119857096</v>
-      </c>
-    </row>
-    <row r="44" spans="3:18" x14ac:dyDescent="0.45">
-      <c r="C44" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D44" s="7">
-        <v>262.08005395366013</v>
-      </c>
-      <c r="E44" s="7">
-        <v>229.18994537957005</v>
-      </c>
-      <c r="F44" s="7">
-        <v>214.41985308647008</v>
-      </c>
-      <c r="G44" s="7">
-        <v>189.14094826942008</v>
-      </c>
-      <c r="H44" s="7">
-        <v>253.93991643427003</v>
-      </c>
-      <c r="I44" s="7">
-        <v>189.51735317766997</v>
-      </c>
-      <c r="J44" s="7">
-        <v>158.94995288181997</v>
-      </c>
-      <c r="K44" s="7">
-        <v>194.97983315401009</v>
-      </c>
-      <c r="L44" s="7">
-        <v>201.47000141185998</v>
-      </c>
-      <c r="M44" s="7">
-        <v>185.39015358801998</v>
-      </c>
-      <c r="N44" s="7">
-        <v>215.90994034904</v>
-      </c>
-      <c r="O44" s="7">
-        <v>75.699891069079996</v>
-      </c>
-      <c r="P44" s="4">
-        <v>2370.68784275489</v>
-      </c>
-    </row>
-    <row r="45" spans="3:18" x14ac:dyDescent="0.45">
-      <c r="C45" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D45" s="7">
-        <v>691.87986686631984</v>
-      </c>
-      <c r="E45" s="7">
-        <v>498.44067769170005</v>
-      </c>
-      <c r="F45" s="7">
-        <v>504.77992710040013</v>
-      </c>
-      <c r="G45" s="7">
-        <v>411.24003005265996</v>
-      </c>
-      <c r="H45" s="7">
-        <v>338.1599618413</v>
-      </c>
-      <c r="I45" s="7">
-        <v>493.46009193824005</v>
-      </c>
-      <c r="J45" s="7">
-        <v>485.86012513887999</v>
-      </c>
-      <c r="K45" s="7">
-        <v>507.17981872393995</v>
-      </c>
-      <c r="L45" s="7">
-        <v>1045.4425698431403</v>
-      </c>
-      <c r="M45" s="7">
-        <v>979.66219994239975</v>
-      </c>
-      <c r="N45" s="7">
-        <v>950.83481948461997</v>
-      </c>
-      <c r="O45" s="7">
-        <v>316.96593782509996</v>
-      </c>
-      <c r="P45" s="4">
-        <v>7223.9060264487007</v>
-      </c>
-    </row>
-    <row r="46" spans="3:18" x14ac:dyDescent="0.45">
-      <c r="C46" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D46" s="7">
-        <v>52.709941031080007</v>
-      </c>
-      <c r="E46" s="7">
-        <v>70.329944243920011</v>
-      </c>
-      <c r="F46" s="7">
-        <v>64.020035235080016</v>
-      </c>
-      <c r="G46" s="7">
-        <v>55.649940110140008</v>
-      </c>
-      <c r="H46" s="7">
-        <v>60.079985776519997</v>
-      </c>
-      <c r="I46" s="7">
-        <v>65.190017650840005</v>
-      </c>
-      <c r="J46" s="7">
-        <v>52.34846451963999</v>
-      </c>
-      <c r="K46" s="7">
-        <v>35.960020007980013</v>
-      </c>
-      <c r="L46" s="7">
-        <v>75.999972250740001</v>
-      </c>
-      <c r="M46" s="7">
-        <v>59.486573096379999</v>
-      </c>
-      <c r="N46" s="7">
-        <v>66.500051909459998</v>
-      </c>
-      <c r="O46" s="7">
-        <v>22.639974944919999</v>
-      </c>
-      <c r="P46" s="4">
-        <v>680.9149207767</v>
-      </c>
-    </row>
-    <row r="47" spans="3:18" x14ac:dyDescent="0.45">
-      <c r="C47" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D47" s="7">
-        <v>265.53037284018006</v>
-      </c>
-      <c r="E47" s="7">
-        <v>298.06031156059998</v>
-      </c>
-      <c r="F47" s="7">
-        <v>277.24026974551998</v>
-      </c>
-      <c r="G47" s="7">
-        <v>234.74977038997</v>
-      </c>
-      <c r="H47" s="7">
-        <v>303.10180842732018</v>
-      </c>
-      <c r="I47" s="7">
-        <v>319.37674114584991</v>
-      </c>
-      <c r="J47" s="7">
-        <v>326.46279450795998</v>
-      </c>
-      <c r="K47" s="7">
-        <v>308.90969839320996</v>
-      </c>
-      <c r="L47" s="7">
-        <v>253.75496100106997</v>
-      </c>
-      <c r="M47" s="7">
-        <v>293.75964522167004</v>
-      </c>
-      <c r="N47" s="7">
-        <v>395.07832636633015</v>
-      </c>
-      <c r="O47" s="7">
-        <v>85.979991121030025</v>
-      </c>
-      <c r="P47" s="4">
-        <v>3362.0046907207106</v>
-      </c>
-    </row>
-    <row r="48" spans="3:18" x14ac:dyDescent="0.45">
-      <c r="C48" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D48" s="7">
-        <v>311.18007212823011</v>
-      </c>
-      <c r="E48" s="7">
-        <v>261.09000536037001</v>
-      </c>
-      <c r="F48" s="7">
-        <v>379.23884784603018</v>
-      </c>
-      <c r="G48" s="7">
-        <v>226.65271922883997</v>
-      </c>
-      <c r="H48" s="7">
-        <v>233.52547702782005</v>
-      </c>
-      <c r="I48" s="7">
-        <v>155.90486697649999</v>
-      </c>
-      <c r="J48" s="7">
-        <v>307.61018325303002</v>
-      </c>
-      <c r="K48" s="7">
-        <v>268.78979718834995</v>
-      </c>
-      <c r="L48" s="7">
-        <v>252.86021551026002</v>
-      </c>
-      <c r="M48" s="7">
-        <v>252.39017191052</v>
-      </c>
-      <c r="N48" s="7">
-        <v>255.16624301435004</v>
-      </c>
-      <c r="O48" s="7">
-        <v>112.85478823388002</v>
-      </c>
-      <c r="P48" s="4">
-        <v>3017.2633876781802</v>
-      </c>
-    </row>
-    <row r="49" spans="3:16" x14ac:dyDescent="0.45">
-      <c r="C49" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D49" s="7">
-        <v>180.07006411553004</v>
-      </c>
-      <c r="E49" s="7">
-        <v>330.01979733371979</v>
-      </c>
-      <c r="F49" s="7">
-        <v>284.75077217346001</v>
-      </c>
-      <c r="G49" s="7">
-        <v>404.19365557087991</v>
-      </c>
-      <c r="H49" s="7">
-        <v>161.68774713933993</v>
-      </c>
-      <c r="I49" s="7">
-        <v>151.84647345754001</v>
-      </c>
-      <c r="J49" s="7">
-        <v>190.14005629174</v>
-      </c>
-      <c r="K49" s="7">
-        <v>160.90988898139005</v>
-      </c>
-      <c r="L49" s="7">
-        <v>201.02993829977999</v>
-      </c>
-      <c r="M49" s="7">
-        <v>135.65001009824996</v>
-      </c>
-      <c r="N49" s="7">
-        <v>164.14999712743003</v>
-      </c>
-      <c r="O49" s="7">
-        <v>67.439168733330007</v>
-      </c>
-      <c r="P49" s="4">
-        <v>2431.8875693223899</v>
-      </c>
-    </row>
-    <row r="50" spans="3:16" x14ac:dyDescent="0.45">
-      <c r="C50" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D50" s="7">
-        <v>147.86567570579999</v>
-      </c>
-      <c r="E50" s="7">
-        <v>248.16798184252008</v>
-      </c>
-      <c r="F50" s="7">
-        <v>209.66001228492001</v>
-      </c>
-      <c r="G50" s="7">
-        <v>231.44775961573009</v>
-      </c>
-      <c r="H50" s="7">
-        <v>215.77983507246</v>
-      </c>
-      <c r="I50" s="7">
-        <v>223.35993857879998</v>
-      </c>
-      <c r="J50" s="7">
-        <v>237.97003435508998</v>
-      </c>
-      <c r="K50" s="7">
-        <v>277.76019594910997</v>
-      </c>
-      <c r="L50" s="7">
-        <v>229.0898086066</v>
-      </c>
-      <c r="M50" s="7">
-        <v>262.07565316116001</v>
-      </c>
-      <c r="N50" s="7">
-        <v>215.34988311985006</v>
-      </c>
-      <c r="O50" s="7">
-        <v>83.339968690769993</v>
-      </c>
-      <c r="P50" s="4">
-        <v>2581.8667469828101</v>
-      </c>
-    </row>
-    <row r="51" spans="3:16" x14ac:dyDescent="0.45">
-      <c r="C51" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D51" s="7">
-        <v>120.08002137007</v>
-      </c>
-      <c r="E51" s="7">
-        <v>119.86008628704997</v>
-      </c>
-      <c r="F51" s="7">
-        <v>95.740525338359987</v>
-      </c>
-      <c r="G51" s="7">
-        <v>145.15700140810003</v>
-      </c>
-      <c r="H51" s="7">
-        <v>69.839946445870012</v>
-      </c>
-      <c r="I51" s="7">
-        <v>94.469987937879978</v>
-      </c>
-      <c r="J51" s="7">
-        <v>121.15000594718002</v>
-      </c>
-      <c r="K51" s="7">
-        <v>100.14620376322003</v>
-      </c>
-      <c r="L51" s="7">
-        <v>105.45511203705001</v>
-      </c>
-      <c r="M51" s="7">
-        <v>103.48997992588004</v>
-      </c>
-      <c r="N51" s="7">
-        <v>121.59998128758001</v>
-      </c>
-      <c r="O51" s="7">
-        <v>58.340010834929998</v>
-      </c>
-      <c r="P51" s="4">
-        <v>1255.3288625831701</v>
-      </c>
-    </row>
-    <row r="52" spans="3:16" x14ac:dyDescent="0.45">
-      <c r="C52" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D52" s="7">
-        <v>231.48972075598999</v>
-      </c>
-      <c r="E52" s="7">
-        <v>227.94882377284006</v>
-      </c>
-      <c r="F52" s="7">
-        <v>230.07500720234</v>
-      </c>
-      <c r="G52" s="7">
-        <v>205.91983226381001</v>
-      </c>
-      <c r="H52" s="7">
-        <v>176.4800002954</v>
-      </c>
-      <c r="I52" s="7">
-        <v>230.71008503998993</v>
-      </c>
-      <c r="J52" s="7">
-        <v>171.09005716741001</v>
-      </c>
-      <c r="K52" s="7">
-        <v>175.2700043575</v>
-      </c>
-      <c r="L52" s="7">
-        <v>179.16318553529007</v>
-      </c>
-      <c r="M52" s="7">
-        <v>219.86020040429997</v>
-      </c>
-      <c r="N52" s="7">
-        <v>248.44490849705005</v>
-      </c>
-      <c r="O52" s="7">
-        <v>50.969955882420003</v>
-      </c>
-      <c r="P52" s="4">
-        <v>2347.4217811743401</v>
-      </c>
-    </row>
-    <row r="53" spans="3:16" x14ac:dyDescent="0.45">
-      <c r="C53" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D53" s="7">
-        <v>53.659965789979985</v>
-      </c>
-      <c r="E53" s="7">
-        <v>58.440010333559997</v>
-      </c>
-      <c r="F53" s="7">
-        <v>61.962507248480016</v>
-      </c>
-      <c r="G53" s="7">
-        <v>61.630983081659991</v>
-      </c>
-      <c r="H53" s="7">
-        <v>69.460040433099991</v>
-      </c>
-      <c r="I53" s="7">
-        <v>87.629993057040011</v>
-      </c>
-      <c r="J53" s="7">
-        <v>71.850026648540009</v>
-      </c>
-      <c r="K53" s="7">
-        <v>75.598962663620014</v>
-      </c>
-      <c r="L53" s="7">
-        <v>65.71998179242</v>
-      </c>
-      <c r="M53" s="7">
-        <v>74.249975354640014</v>
-      </c>
-      <c r="N53" s="7">
-        <v>40.325386038200008</v>
-      </c>
-      <c r="O53" s="7">
-        <v>18.6595733708</v>
-      </c>
-      <c r="P53" s="4">
-        <v>739.18740581203997</v>
-      </c>
-    </row>
-    <row r="54" spans="3:16" x14ac:dyDescent="0.45">
-      <c r="C54" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D54" s="7">
-        <v>301.95002615153993</v>
-      </c>
-      <c r="E54" s="7">
-        <v>217.25978081156001</v>
-      </c>
-      <c r="F54" s="7">
-        <v>220.05630568406002</v>
-      </c>
-      <c r="G54" s="7">
-        <v>245.94320170424007</v>
-      </c>
-      <c r="H54" s="7">
-        <v>272.80239232827995</v>
-      </c>
-      <c r="I54" s="7">
-        <v>235.47988389516007</v>
-      </c>
-      <c r="J54" s="7">
-        <v>189.81998739605001</v>
-      </c>
-      <c r="K54" s="7">
-        <v>231.54995031919006</v>
-      </c>
-      <c r="L54" s="7">
-        <v>345.55797494818995</v>
-      </c>
-      <c r="M54" s="7">
-        <v>265.71987981991003</v>
-      </c>
-      <c r="N54" s="7">
-        <v>222.89164869828008</v>
-      </c>
-      <c r="O54" s="7">
-        <v>76.78987945934</v>
-      </c>
-      <c r="P54" s="4">
-        <v>2825.8209112158002</v>
-      </c>
-    </row>
-    <row r="55" spans="3:16" x14ac:dyDescent="0.45">
-      <c r="C55" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D55" s="7">
-        <v>239.77992403985002</v>
-      </c>
-      <c r="E55" s="7">
-        <v>303.39644565773</v>
-      </c>
-      <c r="F55" s="7">
-        <v>182.37696713533001</v>
-      </c>
-      <c r="G55" s="7">
-        <v>202.76353687854996</v>
-      </c>
-      <c r="H55" s="7">
-        <v>261.78427818379004</v>
-      </c>
-      <c r="I55" s="7">
-        <v>143.32688843436</v>
-      </c>
-      <c r="J55" s="7">
-        <v>155.08991914004002</v>
-      </c>
-      <c r="K55" s="7">
-        <v>148.26144187077</v>
-      </c>
-      <c r="L55" s="7">
-        <v>121.26012858174002</v>
-      </c>
-      <c r="M55" s="7">
-        <v>222.33807766979004</v>
-      </c>
-      <c r="N55" s="7">
-        <v>187.96482171035998</v>
-      </c>
-      <c r="O55" s="7">
-        <v>102.32993641924003</v>
-      </c>
-      <c r="P55" s="4">
-        <v>2270.6723657215498</v>
-      </c>
-    </row>
-    <row r="56" spans="3:16" x14ac:dyDescent="0.45">
-      <c r="C56" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D56" s="4">
-        <v>4756.3877641344397</v>
-      </c>
-      <c r="E56" s="4">
-        <v>4644.7815952145193</v>
-      </c>
-      <c r="F56" s="4">
-        <v>4475.4993585715711</v>
-      </c>
-      <c r="G56" s="4">
-        <v>4217.3341218235091</v>
-      </c>
-      <c r="H56" s="4">
-        <v>4058.9333345804698</v>
-      </c>
-      <c r="I56" s="4">
-        <v>4032.2552300751995</v>
-      </c>
-      <c r="J56" s="4">
-        <v>4069.86879908529</v>
-      </c>
-      <c r="K56" s="4">
-        <v>4005.0637221624297</v>
-      </c>
-      <c r="L56" s="4">
-        <v>4630.8368471926706</v>
-      </c>
-      <c r="M56" s="4">
-        <v>4636.2744064137605</v>
-      </c>
-      <c r="N56" s="4">
-        <v>4283.8975627728514</v>
-      </c>
-      <c r="O56" s="4">
-        <v>1769.32029858185</v>
-      </c>
-      <c r="P56" s="4">
-        <v>49580.453040608554</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="D37:N44">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
-      <formula>100</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="D9:O28">
     <cfRule type="colorScale" priority="4">
       <colorScale>
@@ -3785,22 +2732,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="3" id="{0F9C9A5F-AAD2-41CB-9BBD-5AD3DCCD1657}">
-            <x14:iconSet iconSet="3Triangles">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent">
-                <xm:f>33</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent">
-                <xm:f>67</xm:f>
-              </x14:cfvo>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>D36:O36</xm:sqref>
-        </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{F715C066-47A1-4B39-9614-0E64AEB0F829}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
@@ -3917,19 +2848,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="059fecdb-ee26-4135-81c8-712a955c51df" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="26d2fa48-a9bb-4686-8122-5406e5c0c038">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100265553BD9181624686A68F63ABB446DF" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ee33f439afe5f713e430bc419b9183ba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="26d2fa48-a9bb-4686-8122-5406e5c0c038" xmlns:ns3="059fecdb-ee26-4135-81c8-712a955c51df" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8a55f4bd9fbe5a9e1352735377af3810" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4195,6 +3113,19 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="059fecdb-ee26-4135-81c8-712a955c51df" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="26d2fa48-a9bb-4686-8122-5406e5c0c038">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4205,6 +3136,26 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B64BC13-0F63-452A-A111-F19479EE9CB4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="26d2fa48-a9bb-4686-8122-5406e5c0c038"/>
+    <ds:schemaRef ds:uri="059fecdb-ee26-4135-81c8-712a955c51df"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{72362480-2491-4714-89CC-1BBD7C72E058}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -4224,26 +3175,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B64BC13-0F63-452A-A111-F19479EE9CB4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="26d2fa48-a9bb-4686-8122-5406e5c0c038"/>
-    <ds:schemaRef ds:uri="059fecdb-ee26-4135-81c8-712a955c51df"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{417907D0-8478-4DC5-AA8C-BCF538C18B6A}">
   <ds:schemaRefs>

</xml_diff>